<commit_message>
Fix attributes and casing
Signed-off-by: Adi Bhagavath <adibhagawath@gmail.com>
</commit_message>
<xml_diff>
--- a/docs/Attributesheet_scoring.xlsx
+++ b/docs/Attributesheet_scoring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>Path</t>
   </si>
@@ -105,7 +105,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. ratingType</t>
+      <t>message.rating. rating_type</t>
     </r>
     <r>
       <rPr>
@@ -136,7 +136,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. countOfTxn</t>
+      <t>message.rating. count_of_txn</t>
     </r>
     <r>
       <rPr>
@@ -164,7 +164,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. totalRating</t>
+      <t>message.rating. total_rating</t>
     </r>
     <r>
       <rPr>
@@ -194,9 +194,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>Provider</t>
-  </si>
-  <si>
     <t>IND</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Describes the status of the publish</t>
+  </si>
+  <si>
+    <t>Provider</t>
   </si>
   <si>
     <t>on_publish</t>
@@ -362,7 +362,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. entity_list. ratingType</t>
+      <t>message. entity_list. rating_type</t>
     </r>
     <r>
       <rPr>
@@ -440,7 +440,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. scores. entityName</t>
+      <t>message. scores. entity_name</t>
     </r>
     <r>
       <rPr>
@@ -493,7 +493,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. scores. totalRating</t>
+      <t>message. scores. total_rating</t>
     </r>
     <r>
       <rPr>
@@ -509,28 +509,6 @@
   </si>
   <si>
     <t>Describes the total rating</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>message. scores. countOfTxn</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="11"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>Describes the total number of transactions</t>
@@ -1860,7 +1838,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1641" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.35156" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.6719" style="1" customWidth="1"/>
@@ -2005,223 +1983,223 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="F7" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="12">
+      <c r="F9" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
+      <c r="D12" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="9">
+      <c r="F13" t="s" s="11">
         <v>47</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>48</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="12">
+      <c r="F14" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B16" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="9">
+      <c r="F16" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" ht="12.5" customHeight="1">
       <c r="A17" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s" s="13">
+      <c r="F17" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F17" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -2374,13 +2352,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
         <v>8</v>
@@ -2389,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -2404,124 +2382,124 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="F3" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="F4" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="12">
+      <c r="F5" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="9">
+      <c r="F6" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
+      <c r="D8" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s" s="10">
         <v>25</v>
@@ -2530,97 +2508,97 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>64</v>
       </c>
       <c r="F9" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="12">
+      <c r="F10" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="13">
+      <c r="F13" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -2902,124 +2880,124 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E6" t="s" s="6">
+      <c r="F6" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F6" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="12">
+      <c r="F8" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="9">
+      <c r="F9" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="12.5" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s" s="10">
         <v>25</v>
@@ -3028,97 +3006,97 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>66</v>
       </c>
       <c r="F12" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="12">
+      <c r="F13" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="9">
+      <c r="F14" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B16" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="13">
+      <c r="F16" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F16" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -3173,13 +3151,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
         <v>8</v>
@@ -3188,7 +3166,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -3203,124 +3181,124 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="F3" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="F4" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="12">
+      <c r="F5" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="9">
+      <c r="F6" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
+      <c r="D8" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s" s="10">
         <v>25</v>
@@ -3329,97 +3307,97 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>67</v>
       </c>
       <c r="F9" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="12">
+      <c r="F10" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="13">
+      <c r="F13" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -3661,124 +3639,124 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E4" t="s" s="6">
+      <c r="F4" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F4" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="9">
+      <c r="F5" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="12">
+      <c r="F6" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="9">
+      <c r="F9" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s" s="10">
         <v>25</v>
@@ -3787,97 +3765,97 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="9">
         <v>72</v>
       </c>
       <c r="F10" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="12">
+      <c r="F11" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="9">
+      <c r="F13" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B14" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="13">
+      <c r="F14" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F14" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -4143,7 +4121,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="4">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B6" t="b" s="5">
         <v>1</v>
@@ -4158,7 +4136,7 @@
         <v>150</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -4173,124 +4151,124 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="F7" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="12.5" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="12">
+      <c r="F9" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="12.5" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s" s="10">
         <v>25</v>
@@ -4299,97 +4277,97 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="12">
+      <c r="F14" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B16" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="9">
+      <c r="F16" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" ht="12.5" customHeight="1">
       <c r="A17" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s" s="13">
+      <c r="F17" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F17" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G17" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fix attributes and casing (#76)
</commit_message>
<xml_diff>
--- a/docs/Attributesheet_scoring.xlsx
+++ b/docs/Attributesheet_scoring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>Path</t>
   </si>
@@ -105,7 +105,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. ratingType</t>
+      <t>message.rating. rating_type</t>
     </r>
     <r>
       <rPr>
@@ -136,7 +136,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. countOfTxn</t>
+      <t>message.rating. count_of_txn</t>
     </r>
     <r>
       <rPr>
@@ -164,7 +164,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message.rating. totalRating</t>
+      <t>message.rating. total_rating</t>
     </r>
     <r>
       <rPr>
@@ -194,9 +194,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>Provider</t>
-  </si>
-  <si>
     <t>IND</t>
   </si>
   <si>
@@ -319,6 +316,9 @@
   </si>
   <si>
     <t>Describes the status of the publish</t>
+  </si>
+  <si>
+    <t>Provider</t>
   </si>
   <si>
     <t>on_publish</t>
@@ -362,7 +362,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. entity_list. ratingType</t>
+      <t>message. entity_list. rating_type</t>
     </r>
     <r>
       <rPr>
@@ -440,7 +440,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. scores. entityName</t>
+      <t>message. scores. entity_name</t>
     </r>
     <r>
       <rPr>
@@ -493,7 +493,7 @@
         <color indexed="11"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>message. scores. totalRating</t>
+      <t>message. scores. total_rating</t>
     </r>
     <r>
       <rPr>
@@ -509,28 +509,6 @@
   </si>
   <si>
     <t>Describes the total rating</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="11"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>message. scores. countOfTxn</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="1"/>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="11"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
   </si>
   <si>
     <t>Describes the total number of transactions</t>
@@ -1860,7 +1838,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1641" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.35156" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.6719" style="1" customWidth="1"/>
@@ -2005,223 +1983,223 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="F7" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="12">
+      <c r="F9" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
+      <c r="D12" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="9">
+      <c r="F13" t="s" s="11">
         <v>47</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>48</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="12">
+      <c r="F14" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B16" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="9">
+      <c r="F16" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" ht="12.5" customHeight="1">
       <c r="A17" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s" s="13">
+      <c r="F17" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F17" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -2374,13 +2352,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
         <v>8</v>
@@ -2389,7 +2367,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -2404,124 +2382,124 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="F3" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="F4" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="12">
+      <c r="F5" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="9">
+      <c r="F6" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
+      <c r="D8" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s" s="10">
         <v>25</v>
@@ -2530,97 +2508,97 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>64</v>
       </c>
       <c r="F9" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="12">
+      <c r="F10" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="13">
+      <c r="F13" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -2902,124 +2880,124 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E6" t="s" s="6">
+      <c r="F6" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F6" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="12">
+      <c r="F8" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="9">
+      <c r="F9" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="12.5" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s" s="10">
         <v>25</v>
@@ -3028,97 +3006,97 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>66</v>
       </c>
       <c r="F12" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="12">
+      <c r="F13" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="9">
+      <c r="F14" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B16" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="13">
+      <c r="F16" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F16" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G16" s="3"/>
     </row>
@@ -3173,13 +3151,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="17">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
         <v>8</v>
@@ -3188,7 +3166,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -3203,124 +3181,124 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="F3" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s" s="9">
+      <c r="F4" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E5" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="12">
+      <c r="F5" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="9">
+      <c r="F6" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
+      <c r="D8" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s" s="10">
         <v>25</v>
@@ -3329,97 +3307,97 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>67</v>
       </c>
       <c r="F9" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="12">
+      <c r="F10" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B13" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="13">
+      <c r="F13" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F13" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -3661,124 +3639,124 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E4" t="s" s="6">
+      <c r="F4" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F4" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="9">
+      <c r="F5" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s" s="12">
+      <c r="F6" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s" s="9">
+      <c r="F7" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
+      <c r="D9" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="9">
+      <c r="F9" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s" s="10">
         <v>25</v>
@@ -3787,97 +3765,97 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="9">
         <v>72</v>
       </c>
       <c r="F10" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="12">
+      <c r="F11" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B13" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="9">
+      <c r="F13" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B14" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="13">
+      <c r="F14" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F14" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G14" s="3"/>
     </row>
@@ -4143,7 +4121,7 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="4">
-        <v>82</v>
+        <v>18</v>
       </c>
       <c r="B6" t="b" s="5">
         <v>1</v>
@@ -4158,7 +4136,7 @@
         <v>150</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -4173,124 +4151,124 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="6">
         <v>27</v>
       </c>
-      <c r="E7" t="s" s="6">
+      <c r="F7" t="s" s="8">
         <v>28</v>
-      </c>
-      <c r="F7" t="s" s="8">
-        <v>29</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s" s="9">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s" s="9">
+      <c r="F8" t="s" s="11">
         <v>31</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>32</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" ht="12.5" customHeight="1">
       <c r="A9" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E9" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="B9" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s" s="12">
+      <c r="F9" t="s" s="11">
         <v>34</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>35</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" ht="12.5" customHeight="1">
       <c r="A10" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E10" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="B10" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="9">
+      <c r="F10" t="s" s="11">
         <v>37</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>38</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="12.5" customHeight="1">
       <c r="A11" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B11" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s" s="9">
+      <c r="F11" t="s" s="11">
         <v>40</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>41</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="12.5" customHeight="1">
       <c r="A12" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="B12" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s" s="11">
+      <c r="D12" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s" s="9">
         <v>43</v>
       </c>
-      <c r="D12" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="9">
+      <c r="F12" t="s" s="11">
         <v>44</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>45</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="12.5" customHeight="1">
       <c r="A13" t="s" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s" s="10">
         <v>25</v>
@@ -4299,97 +4277,97 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" ht="12.5" customHeight="1">
       <c r="A14" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E14" t="s" s="12">
         <v>49</v>
       </c>
-      <c r="B14" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s" s="12">
+      <c r="F14" t="s" s="11">
         <v>50</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>51</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" ht="12.5" customHeight="1">
       <c r="A15" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="B15" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="9">
+      <c r="F15" t="s" s="11">
         <v>53</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>54</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" ht="12.5" customHeight="1">
       <c r="A16" t="s" s="9">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s" s="11">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="B16" t="s" s="10">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="D16" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s" s="9">
+      <c r="F16" t="s" s="11">
         <v>56</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>57</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" ht="12.5" customHeight="1">
       <c r="A17" t="s" s="13">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s" s="15">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="B17" t="s" s="14">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s" s="15">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="E17" t="s" s="13">
+      <c r="F17" t="s" s="15">
         <v>59</v>
-      </c>
-      <c r="F17" t="s" s="15">
-        <v>60</v>
       </c>
       <c r="G17" s="3"/>
     </row>

</xml_diff>

<commit_message>
fixes: owner changes in attribute
Signed-off-by: Amar Tumballi <amar@dhiway.com>
</commit_message>
<xml_diff>
--- a/docs/Attributesheet_scoring.xlsx
+++ b/docs/Attributesheet_scoring.xlsx
@@ -61,7 +61,7 @@
     <t>String</t>
   </si>
   <si>
-    <t>Publisher</t>
+    <t>Provider</t>
   </si>
   <si>
     <t>a250a6db99213211f333db7f328085ae277c680d2c7178c4bc65cab9cdab78aa</t>
@@ -315,10 +315,10 @@
     <t>Boolean</t>
   </si>
   <si>
+    <t>Publisher</t>
+  </si>
+  <si>
     <t>Describes the status of the publish</t>
-  </si>
-  <si>
-    <t>Provider</t>
   </si>
   <si>
     <t>on_publish</t>
@@ -1838,7 +1838,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32.1641" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.35156" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.6719" style="1" customWidth="1"/>
@@ -2361,13 +2361,13 @@
         <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -2382,7 +2382,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="6">
         <v>27</v>
@@ -2403,7 +2403,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s" s="9">
         <v>30</v>
@@ -2424,7 +2424,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="12">
         <v>33</v>
@@ -2445,7 +2445,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s" s="9">
         <v>36</v>
@@ -2466,7 +2466,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="9">
         <v>39</v>
@@ -2487,7 +2487,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>43</v>
@@ -2508,7 +2508,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>64</v>
@@ -2529,7 +2529,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="12">
         <v>49</v>
@@ -2550,7 +2550,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>52</v>
@@ -2571,7 +2571,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>55</v>
@@ -2592,7 +2592,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="13">
         <v>58</v>
@@ -3160,13 +3160,13 @@
         <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="6">
         <v>27</v>
@@ -3202,7 +3202,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s" s="9">
         <v>30</v>
@@ -3223,7 +3223,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="12">
         <v>33</v>
@@ -3244,7 +3244,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s" s="9">
         <v>36</v>
@@ -3265,7 +3265,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="9">
         <v>39</v>
@@ -3286,7 +3286,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>43</v>
@@ -3307,7 +3307,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>67</v>
@@ -3328,7 +3328,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="12">
         <v>49</v>
@@ -3349,7 +3349,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>52</v>
@@ -3370,7 +3370,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>55</v>
@@ -3391,7 +3391,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="13">
         <v>58</v>
@@ -4046,7 +4046,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>9</v>
@@ -4067,7 +4067,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s" s="2">
         <v>76</v>
@@ -4088,7 +4088,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5">
         <v>1.5</v>
@@ -4109,7 +4109,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5">
         <v>200</v>
@@ -4130,7 +4130,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5">
         <v>150</v>
@@ -4151,7 +4151,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="6">
         <v>27</v>
@@ -4172,7 +4172,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>30</v>
@@ -4193,7 +4193,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="12">
         <v>33</v>
@@ -4214,7 +4214,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="9">
         <v>36</v>
@@ -4235,7 +4235,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>39</v>
@@ -4256,7 +4256,7 @@
         <v>42</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>43</v>
@@ -4277,7 +4277,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s" s="9">
         <v>83</v>
@@ -4298,7 +4298,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s" s="12">
         <v>49</v>
@@ -4319,7 +4319,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s" s="9">
         <v>52</v>
@@ -4340,7 +4340,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s" s="9">
         <v>55</v>
@@ -4361,7 +4361,7 @@
         <v>26</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s" s="13">
         <v>58</v>

</xml_diff>

<commit_message>
fixes: owner changes in attribute (#77)
Signed-off-by: Amar Tumballi <amar@dhiway.com>
</commit_message>
<xml_diff>
--- a/docs/Attributesheet_scoring.xlsx
+++ b/docs/Attributesheet_scoring.xlsx
@@ -61,7 +61,7 @@
     <t>String</t>
   </si>
   <si>
-    <t>Publisher</t>
+    <t>Provider</t>
   </si>
   <si>
     <t>a250a6db99213211f333db7f328085ae277c680d2c7178c4bc65cab9cdab78aa</t>
@@ -315,10 +315,10 @@
     <t>Boolean</t>
   </si>
   <si>
+    <t>Publisher</t>
+  </si>
+  <si>
     <t>Describes the status of the publish</t>
-  </si>
-  <si>
-    <t>Provider</t>
   </si>
   <si>
     <t>on_publish</t>
@@ -1838,7 +1838,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6667" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="32.1641" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1719" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.6719" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.35156" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.6719" style="1" customWidth="1"/>
@@ -2361,13 +2361,13 @@
         <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" s="2"/>
     </row>
@@ -2382,7 +2382,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="6">
         <v>27</v>
@@ -2403,7 +2403,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s" s="9">
         <v>30</v>
@@ -2424,7 +2424,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="12">
         <v>33</v>
@@ -2445,7 +2445,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s" s="9">
         <v>36</v>
@@ -2466,7 +2466,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="9">
         <v>39</v>
@@ -2487,7 +2487,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>43</v>
@@ -2508,7 +2508,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>64</v>
@@ -2529,7 +2529,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="12">
         <v>49</v>
@@ -2550,7 +2550,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>52</v>
@@ -2571,7 +2571,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>55</v>
@@ -2592,7 +2592,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="13">
         <v>58</v>
@@ -3160,13 +3160,13 @@
         <v>61</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="b" s="5">
         <v>1</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -3181,7 +3181,7 @@
         <v>26</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s" s="6">
         <v>27</v>
@@ -3202,7 +3202,7 @@
         <v>26</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s" s="9">
         <v>30</v>
@@ -3223,7 +3223,7 @@
         <v>26</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s" s="12">
         <v>33</v>
@@ -3244,7 +3244,7 @@
         <v>26</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s" s="9">
         <v>36</v>
@@ -3265,7 +3265,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="9">
         <v>39</v>
@@ -3286,7 +3286,7 @@
         <v>42</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>43</v>
@@ -3307,7 +3307,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>67</v>
@@ -3328,7 +3328,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="12">
         <v>49</v>
@@ -3349,7 +3349,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>52</v>
@@ -3370,7 +3370,7 @@
         <v>26</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>55</v>
@@ -3391,7 +3391,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s" s="13">
         <v>58</v>
@@ -4046,7 +4046,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>9</v>
@@ -4067,7 +4067,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s" s="2">
         <v>76</v>
@@ -4088,7 +4088,7 @@
         <v>22</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5">
         <v>1.5</v>
@@ -4109,7 +4109,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E5" s="5">
         <v>200</v>
@@ -4130,7 +4130,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5">
         <v>150</v>
@@ -4151,7 +4151,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s" s="6">
         <v>27</v>
@@ -4172,7 +4172,7 @@
         <v>26</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>30</v>
@@ -4193,7 +4193,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s" s="12">
         <v>33</v>
@@ -4214,7 +4214,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s" s="9">
         <v>36</v>
@@ -4235,7 +4235,7 @@
         <v>26</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s" s="9">
         <v>39</v>
@@ -4256,7 +4256,7 @@
         <v>42</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s" s="9">
         <v>43</v>
@@ -4277,7 +4277,7 @@
         <v>26</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s" s="9">
         <v>83</v>
@@ -4298,7 +4298,7 @@
         <v>26</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s" s="12">
         <v>49</v>
@@ -4319,7 +4319,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s" s="9">
         <v>52</v>
@@ -4340,7 +4340,7 @@
         <v>26</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s" s="9">
         <v>55</v>
@@ -4361,7 +4361,7 @@
         <v>26</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s" s="13">
         <v>58</v>

</xml_diff>